<commit_message>
Edit downup 300 names file for clarity
Visuals for every sweep direction, errors unfixed
</commit_message>
<xml_diff>
--- a/ARP data/downup/names_0112_downup_300.xlsx
+++ b/ARP data/downup/names_0112_downup_300.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wahlm\OneDrive\Documents\School\Research\ARP\ARPdb\ARP data\downup\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>background</t>
   </si>
@@ -60,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,7 +379,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -384,16 +389,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,12 +406,12 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -417,12 +422,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -430,345 +435,341 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <f>A6+20</f>
-        <v>30</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <f t="shared" ref="A8:A31" si="0">A7+20</f>
-        <v>50</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <f t="shared" si="0"/>
-        <v>70</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
-        <f>A10+20</f>
+        <f>110</f>
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A8:A31" si="0">A17+20</f>
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>230</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>-10</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33">
         <f>A32-20</f>
         <v>-30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" ref="A34:A56" si="1">A33-20</f>
         <v>-50</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>-70</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>-90</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>-110</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>-130</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>-150</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>-170</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>-190</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>-210</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>-230</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>-250</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>-270</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>-290</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>-310</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>-330</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>-350</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>-370</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>-390</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>-410</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>-430</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>-450</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>-470</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>-490</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>410</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>430</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>450</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>470</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>490</v>
       </c>

</xml_diff>